<commit_message>
Update main, create json.file, create csv and create excel
</commit_message>
<xml_diff>
--- a/scraping-data-Jobstreet.xlsx
+++ b/scraping-data-Jobstreet.xlsx
@@ -17,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +45,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,14 +425,906 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Postions</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Company</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Location</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Salary</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Time apply</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>PT. TRANSMORA KREASI NUSANTARA</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Jakarta Raya</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Rp 6.500.000 – Rp 8.500.000 per month</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>3 jam yang lalu</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>PT Infolog Solutions Indonesia</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Jakarta Raya</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Rp 8.000.000 – Rp 12.000.000 per month</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>30+ hari yang lalu</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Assistant software Engineer - Intern (Paid Internship)</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>HITHINK TECHNOLOGY INDONESIA</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Jakarta Selatan</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Salary not found</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>11 jam yang lalu</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Software Engineer I, Backend (Flight)</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>PT Global Tiket Network</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Jakarta Raya</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Salary not found</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>10 jam yang lalu</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Software Engineer, Backend</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>PT Solusi Transportasi Indonesia</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Kebayoran Lama</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Salary not found</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>1 hari yang lalu</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>PT Adecco Personnel Indonesia</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Jakarta Raya</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Salary not found</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>9 hari yang lalu</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Senior Software Engineer - GO, Java, Sprinboot</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>PT XL Axiata Tbk</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Jakarta Raya</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Salary not found</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>2 hari yang lalu</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Software Developer</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>KSP Serambi Dana</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Pasar Minggu</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Rp 5.500.000 – Rp 8.000.000 per month</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>10 hari yang lalu</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>IT Java Developer</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>PT Bank IBK Indonesia, Tbk</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Jakarta Pusat</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Salary not found</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>5 jam yang lalu</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Senior Full Stack Developer</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>PT Datacaraka Solusindo</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Jakarta Raya</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Rp 17.000.000 – Rp 21.000.000 per month</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>4 jam yang lalu</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>ICT Support Services Engineer</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>PT Petrolink Services Indonesia</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Jakarta Raya</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Salary not found</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>14 hari yang lalu</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>PT Aplikasi Karya Anak Bangsa (GO-JEK Indonesia)</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Jakarta Raya</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Salary not found</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>14 hari yang lalu</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>AIF - AHM - Software Engineer Intern</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>PT Astra Honda Motor (Head Office)</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Jakarta Raya</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Salary not found</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>9 hari yang lalu</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Senior Software Engineer in Test (SDET)</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>PT BLANKA JAYA INDONESIA</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Jakarta Selatan</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Rp 20.000.000 – Rp 30.000.000 per month</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>27 hari yang lalu</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Software Engineer I, Frontend (Accommodation)</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>PT Global Tiket Network</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Jakarta Raya</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Salary not found</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>30+ hari yang lalu</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Senior Web &amp; App Developer- Work From Home Basic</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>COOPER SERVICES SDN. BHD.</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Jakarta Raya</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Rp 11,000,000 – Rp 13,000,000 per month</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>7 hari yang lalu</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Fullstack Engineer</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>PT METRA DIGITAL MEDIA BY TELKOM INDONESIA</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Jakarta Selatan</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Salary not found</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>8 hari yang lalu</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Middle Full Stack Developer</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>PT Datacaraka Solusindo</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Jakarta Raya</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Rp 7.800.000 – Rp 10.000.000 per month</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>2 hari yang lalu</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Senior Software Engineer, Backend - Consumer Experience</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>PT Solusi Transportasi Indonesia</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Jakarta Raya</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Salary not found</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>6 hari yang lalu</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Lead Software Engineer</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>PT Aplikasi Karya Anak Bangsa (GO-JEK Indonesia)</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Jakarta Raya</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Salary not found</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>30+ hari yang lalu</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Software Engineer (Java)</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>PT Karisma Zona Kreatifku</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Jakarta Selatan</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Rp 8.000.000 – Rp 12.000.000 per month</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>7 hari yang lalu</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>IT Software Engineer Staff (Software Developer)</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>PT WOORI FINANCE INDONESIA TBK</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Jakarta Raya</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>IDR 5,000,000 - 7,000,000</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>3 hari yang lalu</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>PT Aplikasi Karya Anak Bangsa (GO-JEK Indonesia)</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Jakarta Raya</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Salary not found</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>28 hari yang lalu</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>PROGRAMMER JAVA</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>PT. PLANA NETWORKS INDONESIA</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Jakarta Selatan</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Salary not found</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>16 hari yang lalu</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Senior Software Engineer, Backend (Payments Experience)</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>PT Solusi Transportasi Indonesia</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Jakarta Raya</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Salary not found</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>28 hari yang lalu</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Software Engineer Oracle</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>PT Trinusa Travelindo</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Jakarta Raya</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Salary not found</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>30+ hari yang lalu</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Software Engineer, Fullstack - Payments Experience</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>PT Solusi Transportasi Indonesia</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Sawah Besar</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Salary not found</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>26 hari yang lalu</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>PT SOD Technology Indonesia</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Jakarta Raya</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Salary not found</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>20 hari yang lalu</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>PRODUCT &amp; TECH MANAGER</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>PT. Pasifik Sukses Gemilang</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Jakarta Raya</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Rp 10.000.000 – Rp 13.000.000 per month</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>9 hari yang lalu</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Full Stack Developer (AI Centric)</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>POINTSTAR (PSID)</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Jakarta Raya</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Salary not found</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>17 hari yang lalu</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Senior Software Engineer</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>PT Aplikasi Karya Anak Bangsa (GO-JEK Indonesia)</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Jakarta Raya</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Salary not found</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>30+ hari yang lalu</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Lead Software Engineer, Fullstack</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>PT Solusi Transportasi Indonesia</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Sawah Besar</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Salary not found</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>9 hari yang lalu</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>